<commit_message>
Added messages to owner container to azure storage map
</commit_message>
<xml_diff>
--- a/Azure Storage Account Map.xlsx
+++ b/Azure Storage Account Map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TaHan\Downloads\Apex-Visual-2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tihanewi\Downloads\ApexVisual.F1_2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10E6D6F-495D-4041-9CFC-0E63CE570D85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A049497C-F57A-4953-94EF-40D4E574E95B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3612" yWindow="840" windowWidth="17508" windowHeight="10692" xr2:uid="{B8006B69-B989-4F9B-ABBC-61625677C1A0}"/>
+    <workbookView xWindow="45735" yWindow="735" windowWidth="21600" windowHeight="11145" xr2:uid="{B8006B69-B989-4F9B-ABBC-61625677C1A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Containers" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>Container Name</t>
   </si>
@@ -111,6 +111,15 @@
   </si>
   <si>
     <t>YYYY.MM.DD (i.e. "2020-8-2", 2020-8-16")</t>
+  </si>
+  <si>
+    <t>messagestodeveloper</t>
+  </si>
+  <si>
+    <t>Contains a series of messages to owner.</t>
+  </si>
+  <si>
+    <t>YYYY.MM.DD.HH.MM.SS</t>
   </si>
 </sst>
 </file>
@@ -486,21 +495,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE5C40B7-953D-434C-8823-1D3A499E1342}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="12.33203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="37.109375" customWidth="1"/>
+    <col min="3" max="3" width="37.1328125" customWidth="1"/>
     <col min="4" max="4" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -514,7 +523,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -528,7 +537,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -542,7 +551,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -556,7 +565,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -570,7 +579,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -584,7 +593,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
@@ -598,7 +607,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
@@ -610,6 +619,20 @@
       </c>
       <c r="D8" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated note about wallpapers container
</commit_message>
<xml_diff>
--- a/Azure Storage Account Map.xlsx
+++ b/Azure Storage Account Map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tihanewi\Downloads\ApexVisual.F1_2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A049497C-F57A-4953-94EF-40D4E574E95B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C30B31B-A9A9-45FD-970C-41C56E805F32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45735" yWindow="735" windowWidth="21600" windowHeight="11145" xr2:uid="{B8006B69-B989-4F9B-ABBC-61625677C1A0}"/>
   </bookViews>
@@ -95,9 +95,6 @@
     <t>(none)</t>
   </si>
   <si>
-    <t>All of the wallpaper images that could appear as the background of the home screen</t>
-  </si>
-  <si>
     <t>The unique session ID</t>
   </si>
   <si>
@@ -120,6 +117,9 @@
   </si>
   <si>
     <t>YYYY.MM.DD.HH.MM.SS</t>
+  </si>
+  <si>
+    <t>All of the wallpaper images that could appear as the background of the home screen. This folder still exists but is not being used anymore.</t>
   </si>
 </sst>
 </file>
@@ -498,7 +498,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -534,7 +534,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
@@ -548,7 +548,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
@@ -562,7 +562,7 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
@@ -576,7 +576,7 @@
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
@@ -601,7 +601,7 @@
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
         <v>19</v>
@@ -612,13 +612,13 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
         <v>23</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>24</v>
-      </c>
-      <c r="D8" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
@@ -626,13 +626,13 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
         <v>26</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>27</v>
-      </c>
-      <c r="D9" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated name of container
</commit_message>
<xml_diff>
--- a/Azure Storage Account Map.xlsx
+++ b/Azure Storage Account Map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tihanewi\Downloads\ApexVisual.F1_2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C30B31B-A9A9-45FD-970C-41C56E805F32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1E9419-0F9A-476E-ABF2-7B6C5A7016CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45735" yWindow="735" windowWidth="21600" windowHeight="11145" xr2:uid="{B8006B69-B989-4F9B-ABBC-61625677C1A0}"/>
   </bookViews>
@@ -110,9 +110,6 @@
     <t>YYYY.MM.DD (i.e. "2020-8-2", 2020-8-16")</t>
   </si>
   <si>
-    <t>messagestodeveloper</t>
-  </si>
-  <si>
     <t>Contains a series of messages to owner.</t>
   </si>
   <si>
@@ -120,6 +117,9 @@
   </si>
   <si>
     <t>All of the wallpaper images that could appear as the background of the home screen. This folder still exists but is not being used anymore.</t>
+  </si>
+  <si>
+    <t>messagesubmissions</t>
   </si>
 </sst>
 </file>
@@ -498,7 +498,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -601,7 +601,7 @@
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
         <v>19</v>
@@ -626,13 +626,13 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
         <v>25</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>26</v>
-      </c>
-      <c r="D9" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Azure Storage Account Map
</commit_message>
<xml_diff>
--- a/Azure Storage Account Map.xlsx
+++ b/Azure Storage Account Map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tihanewi\Downloads\ApexVisual.F1_2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1E9419-0F9A-476E-ABF2-7B6C5A7016CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DFF00F-F999-47EF-9223-2DB76F0D772A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45735" yWindow="735" windowWidth="21600" windowHeight="11145" xr2:uid="{B8006B69-B989-4F9B-ABBC-61625677C1A0}"/>
+    <workbookView xWindow="51765" yWindow="2775" windowWidth="16875" windowHeight="10530" xr2:uid="{B8006B69-B989-4F9B-ABBC-61625677C1A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Containers" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>Container Name</t>
   </si>
@@ -89,12 +89,6 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>wallpapers</t>
-  </si>
-  <si>
-    <t>(none)</t>
-  </si>
-  <si>
     <t>The unique session ID</t>
   </si>
   <si>
@@ -107,19 +101,16 @@
     <t>Contains the activity logs for the session. Each day will have its own file, which will be an append blob. Blob name format will be YYYY.MM.DD (i.e. "2020.8.5".  The append blobs will have an activity log split by "&lt;:::SPLIT:::&gt;".</t>
   </si>
   <si>
-    <t>YYYY.MM.DD (i.e. "2020-8-2", 2020-8-16")</t>
-  </si>
-  <si>
     <t>Contains a series of messages to owner.</t>
   </si>
   <si>
-    <t>YYYY.MM.DD.HH.MM.SS</t>
-  </si>
-  <si>
-    <t>All of the wallpaper images that could appear as the background of the home screen. This folder still exists but is not being used anymore.</t>
-  </si>
-  <si>
     <t>messagesubmissions</t>
+  </si>
+  <si>
+    <t>YYYY.MM.DD</t>
+  </si>
+  <si>
+    <t>YYYY.MM.DD (i.e. "2020.8.2", 2020.8.16")</t>
   </si>
 </sst>
 </file>
@@ -495,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE5C40B7-953D-434C-8823-1D3A499E1342}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -534,7 +525,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
@@ -548,7 +539,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
@@ -562,7 +553,7 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
@@ -576,7 +567,7 @@
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
@@ -598,13 +589,13 @@
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
@@ -612,27 +603,13 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
         <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
       </c>
       <c r="D8" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>